<commit_message>
Update tableAUCs to not use bootstrapping
</commit_message>
<xml_diff>
--- a/figures/overlap.xlsx
+++ b/figures/overlap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aubre\Documents\BU Research\tbsp_malnutrition\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875BA0D-779D-4835-93C8-0D0F40FE69E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92769F99-83B4-495B-97BA-B3EE47A38E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="39" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="49" workbookViewId="0">
+      <selection activeCell="BB32" sqref="BB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update gene overlap table (worksheet file)
</commit_message>
<xml_diff>
--- a/figures/overlap.xlsx
+++ b/figures/overlap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aubre\Documents\BU Research\tbsp_malnutrition\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1CD782-E479-4D50-BBEA-063D40205767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6900CEB-6834-459B-811A-BCD447A6082D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="49" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>